<commit_message>
Stripes for "TOO_LOW_TESTING" countries.
</commit_message>
<xml_diff>
--- a/covid.xlsx
+++ b/covid.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,20 +450,25 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>HasLowTesting</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>LastUpdate</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>NotificationRatePer100000</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>PositiveRate</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>TestsPer100000</t>
         </is>
@@ -480,16 +485,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>147.9949999999997</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>9.909970899065669</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>652.8999999999996</v>
       </c>
     </row>
@@ -504,16 +512,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="n">
         <v>44291</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>899.5017000000022</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>9.688263761413223</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>4194.700000000012</v>
       </c>
     </row>
@@ -528,16 +539,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>44295</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>288.6637999999999</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.7989497761960898</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>17224.90000000002</v>
       </c>
     </row>
@@ -552,16 +566,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="n">
         <v>44289</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>495.5440999999999</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>55.48245582401741</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>554.5999999999992</v>
       </c>
     </row>
@@ -576,16 +593,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>421.8364999999998</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>20.73096870342772</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>1006.5</v>
       </c>
     </row>
@@ -600,16 +620,19 @@
           <t>GREEN</t>
         </is>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>0.5607999999999947</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>0.02072079747806103</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>1173.699999999997</v>
       </c>
     </row>
@@ -624,16 +647,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>450.1466</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>0.8840993268563807</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>22922.3</v>
       </c>
     </row>
@@ -648,16 +674,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>472.1381999999998</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>7.411614442612031</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>2849.900000000002</v>
       </c>
     </row>
@@ -669,19 +698,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="n">
+          <t>RED</t>
+        </is>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>54.06669999999995</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>21.833535660091</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>131.8000000000001</v>
       </c>
     </row>
@@ -696,16 +728,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="n">
         <v>44295</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>622.2974999999999</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>17.95324445028242</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>1522.6</v>
       </c>
     </row>
@@ -720,16 +755,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="n">
         <v>44295</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>859.0236000000004</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>6.089226661606881</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>7378.399999999965</v>
       </c>
     </row>
@@ -744,16 +782,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>606.4041999999994</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>25.32973345136222</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>1016.7</v>
       </c>
     </row>
@@ -768,16 +809,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>183.6851999999999</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>8.092977847824221</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>1142.099999999994</v>
       </c>
     </row>
@@ -792,16 +836,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>106.8017</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>15.68964194373403</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>390.9999999999997</v>
       </c>
     </row>
@@ -816,16 +863,19 @@
           <t>NO_DATA</t>
         </is>
       </c>
-      <c r="C16" s="2" t="n">
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="n">
         <v>44093</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>445.6800999999999</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>95.33163473298006</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>245.3</v>
       </c>
     </row>
@@ -840,16 +890,19 @@
           <t>NO_DATA</t>
         </is>
       </c>
-      <c r="C17" s="2" t="n">
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="n">
         <v>44281</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>5.961500000000001</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>0.2040587823652926</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>1714.799999999991</v>
       </c>
     </row>
@@ -864,16 +917,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C18" s="2" t="n">
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>258.8591</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>7.312733486259972</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>2136.10000000001</v>
       </c>
     </row>
@@ -888,16 +944,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C19" s="2" t="n">
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>292.6298999999999</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>5.621528830050252</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>2507.800000000009</v>
       </c>
     </row>
@@ -912,16 +971,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C20" s="2" t="n">
+      <c r="C20" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>519.2241999999999</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>12.57309998066131</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>2068.400000000008</v>
       </c>
     </row>
@@ -933,19 +995,22 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C21" s="2" t="n">
+          <t>GREEN</t>
+        </is>
+      </c>
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>7.680600000000004</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>2.087349397590371</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>82.99999999999983</v>
       </c>
     </row>
@@ -957,19 +1022,22 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="n">
+          <t>ORANGE</t>
+        </is>
+      </c>
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>0.683299999999997</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>17.30714285714287</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>1.4</v>
       </c>
     </row>
@@ -984,16 +1052,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C23" s="2" t="n">
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
         <v>301.6103000000003</v>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>28.23495130129347</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>626.2999999999977</v>
       </c>
     </row>
@@ -1008,16 +1079,19 @@
           <t>NO_DATA</t>
         </is>
       </c>
-      <c r="C24" s="2" t="n">
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="n">
         <v>44175</v>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
         <v>338.1367999999999</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>50.01500735654736</v>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>407.8</v>
       </c>
     </row>
@@ -1032,16 +1106,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C25" s="2" t="n">
+      <c r="C25" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="n">
         <v>44292</v>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
         <v>144.5983</v>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>23.2795034878949</v>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>487.3999999999995</v>
       </c>
     </row>
@@ -1056,16 +1133,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C26" s="2" t="n">
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>123.8498</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>4.846519484600875</v>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>1272.800000000001</v>
       </c>
     </row>
@@ -1080,16 +1160,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C27" s="2" t="n">
+      <c r="C27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
         <v>784.7937000000005</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>1.045229156456049</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>41419.30000000002</v>
       </c>
     </row>
@@ -1104,16 +1187,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C28" s="2" t="n">
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
         <v>608.4611999999994</v>
       </c>
-      <c r="E28" t="n">
+      <c r="F28" t="n">
         <v>3.310430032076999</v>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>7980.800000000001</v>
       </c>
     </row>
@@ -1128,16 +1214,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C29" s="2" t="n">
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2" t="n">
         <v>44290</v>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
         <v>271.5388999999996</v>
       </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
         <v>10.07853029087995</v>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>1371.699999999998</v>
       </c>
     </row>
@@ -1152,16 +1241,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C30" s="2" t="n">
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2" t="n">
         <v>44292</v>
       </c>
-      <c r="D30" t="n">
+      <c r="E30" t="n">
         <v>168.8304000000004</v>
       </c>
-      <c r="E30" t="n">
+      <c r="F30" t="n">
         <v>0.3966080634229527</v>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>19475.59999999998</v>
       </c>
     </row>
@@ -1173,19 +1265,22 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C31" s="2" t="n">
+          <t>RED</t>
+        </is>
+      </c>
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2" t="n">
         <v>44289</v>
       </c>
-      <c r="D31" t="n">
+      <c r="E31" t="n">
         <v>52.68300000000018</v>
       </c>
-      <c r="E31" t="n">
+      <c r="F31" t="n">
         <v>18.49652122641517</v>
       </c>
-      <c r="F31" t="n">
+      <c r="G31" t="n">
         <v>169.5999999999998</v>
       </c>
     </row>
@@ -1197,19 +1292,22 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C32" s="2" t="n">
+          <t>RED</t>
+        </is>
+      </c>
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2" t="n">
         <v>44289</v>
       </c>
-      <c r="D32" t="n">
+      <c r="E32" t="n">
         <v>126.5937000000002</v>
       </c>
-      <c r="E32" t="n">
+      <c r="F32" t="n">
         <v>37.1940483205657</v>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>169.7000000000003</v>
       </c>
     </row>
@@ -1224,16 +1322,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C33" s="2" t="n">
+      <c r="C33" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2" t="n">
         <v>44287</v>
       </c>
-      <c r="D33" t="n">
+      <c r="E33" t="n">
         <v>197.1734000000011</v>
       </c>
-      <c r="E33" t="n">
+      <c r="F33" t="n">
         <v>6.673969296775554</v>
       </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>1491.700000000003</v>
       </c>
     </row>
@@ -1248,16 +1349,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C34" s="2" t="n">
+      <c r="C34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D34" t="n">
+      <c r="E34" t="n">
         <v>794.8504</v>
       </c>
-      <c r="E34" t="n">
+      <c r="F34" t="n">
         <v>15.2286373059187</v>
       </c>
-      <c r="F34" t="n">
+      <c r="G34" t="n">
         <v>2363.699999999994</v>
       </c>
     </row>
@@ -1269,19 +1373,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C35" s="2" t="n">
+          <t>ORANGE</t>
+        </is>
+      </c>
+      <c r="C35" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D35" t="n">
+      <c r="E35" t="n">
         <v>24.73210000000001</v>
       </c>
-      <c r="E35" t="n">
+      <c r="F35" t="n">
         <v>23.97185628742512</v>
       </c>
-      <c r="F35" t="n">
+      <c r="G35" t="n">
         <v>50.10000000000012</v>
       </c>
     </row>
@@ -1296,16 +1403,19 @@
           <t>ORANGE</t>
         </is>
       </c>
-      <c r="C36" s="2" t="n">
+      <c r="C36" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D36" t="n">
+      <c r="E36" t="n">
         <v>109.1917000000001</v>
       </c>
-      <c r="E36" t="n">
+      <c r="F36" t="n">
         <v>2.870299874304191</v>
       </c>
-      <c r="F36" t="n">
+      <c r="G36" t="n">
         <v>1670.699999999999</v>
       </c>
     </row>
@@ -1317,19 +1427,22 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C37" s="2" t="n">
+          <t>GREEN</t>
+        </is>
+      </c>
+      <c r="C37" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D37" t="n">
+      <c r="E37" t="n">
         <v>0.1115000000000009</v>
       </c>
-      <c r="E37" t="n">
+      <c r="F37" t="n">
         <v>0.05457660303475328</v>
       </c>
-      <c r="F37" t="n">
+      <c r="G37" t="n">
         <v>204.2999999999999</v>
       </c>
     </row>
@@ -1344,16 +1457,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C38" s="2" t="n">
+      <c r="C38" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="2" t="n">
         <v>44291</v>
       </c>
-      <c r="D38" t="n">
+      <c r="E38" t="n">
         <v>753.3637000000002</v>
       </c>
-      <c r="E38" t="n">
+      <c r="F38" t="n">
         <v>7.499777326184732</v>
       </c>
-      <c r="F38" t="n">
+      <c r="G38" t="n">
         <v>4625.599999999999</v>
       </c>
     </row>
@@ -1368,16 +1484,19 @@
           <t>ORANGE</t>
         </is>
       </c>
-      <c r="C39" s="2" t="n">
+      <c r="C39" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D39" t="n">
+      <c r="E39" t="n">
         <v>55.3826000000001</v>
       </c>
-      <c r="E39" t="n">
+      <c r="F39" t="n">
         <v>0.1913117117117115</v>
       </c>
-      <c r="F39" t="n">
+      <c r="G39" t="n">
         <v>8325</v>
       </c>
     </row>
@@ -1389,19 +1508,22 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C40" s="2" t="n">
+          <t>GREEN</t>
+        </is>
+      </c>
+      <c r="C40" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" s="2" t="n">
         <v>44289</v>
       </c>
-      <c r="D40" t="n">
+      <c r="E40" t="n">
         <v>3.13130000000001</v>
       </c>
-      <c r="E40" t="n">
+      <c r="F40" t="n">
         <v>2.30284431137722</v>
       </c>
-      <c r="F40" t="n">
+      <c r="G40" t="n">
         <v>66.79999999999993</v>
       </c>
     </row>
@@ -1416,16 +1538,19 @@
           <t>NO_DATA</t>
         </is>
       </c>
-      <c r="C41" s="2" t="n">
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" s="2" t="n">
         <v>44270</v>
       </c>
-      <c r="D41" t="n">
+      <c r="E41" t="n">
         <v>8.317300000000023</v>
       </c>
-      <c r="E41" t="n">
+      <c r="F41" t="n">
         <v>4.57673888255414</v>
       </c>
-      <c r="F41" t="n">
+      <c r="G41" t="n">
         <v>87.70000000000024</v>
       </c>
     </row>
@@ -1440,16 +1565,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C42" s="2" t="n">
+      <c r="C42" t="b">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D42" t="n">
+      <c r="E42" t="n">
         <v>397.6665000000001</v>
       </c>
-      <c r="E42" t="n">
+      <c r="F42" t="n">
         <v>5.859195909547435</v>
       </c>
-      <c r="F42" t="n">
+      <c r="G42" t="n">
         <v>3285.699999999997</v>
       </c>
     </row>
@@ -1461,19 +1589,22 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C43" s="2" t="n">
+          <t>RED</t>
+        </is>
+      </c>
+      <c r="C43" t="b">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D43" t="n">
+      <c r="E43" t="n">
         <v>54.10939999999992</v>
       </c>
-      <c r="E43" t="n">
+      <c r="F43" t="n">
         <v>22.0599063962558</v>
       </c>
-      <c r="F43" t="n">
+      <c r="G43" t="n">
         <v>192.3000000000002</v>
       </c>
     </row>
@@ -1488,16 +1619,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C44" s="2" t="n">
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2" t="n">
         <v>44295</v>
       </c>
-      <c r="D44" t="n">
+      <c r="E44" t="n">
         <v>616.1350999999995</v>
       </c>
-      <c r="E44" t="n">
+      <c r="F44" t="n">
         <v>24.18851963746218</v>
       </c>
-      <c r="F44" t="n">
+      <c r="G44" t="n">
         <v>1257.800000000003</v>
       </c>
     </row>
@@ -1512,16 +1646,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C45" s="2" t="n">
+      <c r="C45" t="b">
+        <v>0</v>
+      </c>
+      <c r="D45" s="2" t="n">
         <v>44295</v>
       </c>
-      <c r="D45" t="n">
+      <c r="E45" t="n">
         <v>893.3735</v>
       </c>
-      <c r="E45" t="n">
+      <c r="F45" t="n">
         <v>19.90713321332136</v>
       </c>
-      <c r="F45" t="n">
+      <c r="G45" t="n">
         <v>1777.599999999995</v>
       </c>
     </row>
@@ -1533,19 +1670,22 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C46" s="2" t="n">
+          <t>ORANGE</t>
+        </is>
+      </c>
+      <c r="C46" t="b">
+        <v>1</v>
+      </c>
+      <c r="D46" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D46" t="n">
+      <c r="E46" t="n">
         <v>25.92460000000001</v>
       </c>
-      <c r="E46" t="n">
+      <c r="F46" t="n">
         <v>10.6586821015138</v>
       </c>
-      <c r="F46" t="n">
+      <c r="G46" t="n">
         <v>112.3000000000001</v>
       </c>
     </row>
@@ -1560,16 +1700,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C47" s="2" t="n">
+      <c r="C47" t="b">
+        <v>0</v>
+      </c>
+      <c r="D47" s="2" t="n">
         <v>44295</v>
       </c>
-      <c r="D47" t="n">
+      <c r="E47" t="n">
         <v>107.8309999999999</v>
       </c>
-      <c r="E47" t="n">
+      <c r="F47" t="n">
         <v>11.54607027669328</v>
       </c>
-      <c r="F47" t="n">
+      <c r="G47" t="n">
         <v>589.0999999999991</v>
       </c>
     </row>
@@ -1584,16 +1727,19 @@
           <t>ORANGE</t>
         </is>
       </c>
-      <c r="C48" s="2" t="n">
+      <c r="C48" t="b">
+        <v>0</v>
+      </c>
+      <c r="D48" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D48" t="n">
+      <c r="E48" t="n">
         <v>129.6934999999998</v>
       </c>
-      <c r="E48" t="n">
+      <c r="F48" t="n">
         <v>2.526525423728806</v>
       </c>
-      <c r="F48" t="n">
+      <c r="G48" t="n">
         <v>2242.000000000007</v>
       </c>
     </row>
@@ -1608,16 +1754,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C49" s="2" t="n">
+      <c r="C49" t="b">
+        <v>0</v>
+      </c>
+      <c r="D49" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D49" t="n">
+      <c r="E49" t="n">
         <v>255.3392</v>
       </c>
-      <c r="E49" t="n">
+      <c r="F49" t="n">
         <v>27.10738786279683</v>
       </c>
-      <c r="F49" t="n">
+      <c r="G49" t="n">
         <v>606.3999999999993</v>
       </c>
     </row>
@@ -1632,16 +1781,19 @@
           <t>NO_DATA</t>
         </is>
       </c>
-      <c r="C50" s="2" t="n">
+      <c r="C50" t="b">
+        <v>0</v>
+      </c>
+      <c r="D50" s="2" t="n">
         <v>44284</v>
       </c>
-      <c r="D50" t="n">
+      <c r="E50" t="n">
         <v>230.0155999999999</v>
       </c>
-      <c r="E50" t="n">
+      <c r="F50" t="n">
         <v>19.11048773189709</v>
       </c>
-      <c r="F50" t="n">
+      <c r="G50" t="n">
         <v>668.3999999999997</v>
       </c>
     </row>
@@ -1656,16 +1808,19 @@
           <t>ORANGE</t>
         </is>
       </c>
-      <c r="C51" s="2" t="n">
+      <c r="C51" t="b">
+        <v>0</v>
+      </c>
+      <c r="D51" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D51" t="n">
+      <c r="E51" t="n">
         <v>27.83889999999992</v>
       </c>
-      <c r="E51" t="n">
+      <c r="F51" t="n">
         <v>0.4449434066439577</v>
       </c>
-      <c r="F51" t="n">
+      <c r="G51" t="n">
         <v>2173.400000000004</v>
       </c>
     </row>
@@ -1680,16 +1835,19 @@
           <t>ORANGE</t>
         </is>
       </c>
-      <c r="C52" s="2" t="n">
+      <c r="C52" t="b">
+        <v>0</v>
+      </c>
+      <c r="D52" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D52" t="n">
+      <c r="E52" t="n">
         <v>46.3172000000006</v>
       </c>
-      <c r="E52" t="n">
+      <c r="F52" t="n">
         <v>0.5745649224234716</v>
       </c>
-      <c r="F52" t="n">
+      <c r="G52" t="n">
         <v>3390.199999999982</v>
       </c>
     </row>
@@ -1704,16 +1862,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C53" s="2" t="n">
+      <c r="C53" t="b">
+        <v>0</v>
+      </c>
+      <c r="D53" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D53" t="n">
+      <c r="E53" t="n">
         <v>393.2349000000002</v>
       </c>
-      <c r="E53" t="n">
+      <c r="F53" t="n">
         <v>5.462022764227642</v>
       </c>
-      <c r="F53" t="n">
+      <c r="G53" t="n">
         <v>3075</v>
       </c>
     </row>
@@ -1728,16 +1889,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C54" s="2" t="n">
+      <c r="C54" t="b">
+        <v>0</v>
+      </c>
+      <c r="D54" s="2" t="n">
         <v>44288</v>
       </c>
-      <c r="D54" t="n">
+      <c r="E54" t="n">
         <v>144.3014999999999</v>
       </c>
-      <c r="E54" t="n">
+      <c r="F54" t="n">
         <v>11.65880473595189</v>
       </c>
-      <c r="F54" t="n">
+      <c r="G54" t="n">
         <v>532.0999999999998</v>
       </c>
     </row>
@@ -1752,16 +1916,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C55" s="2" t="n">
+      <c r="C55" t="b">
+        <v>0</v>
+      </c>
+      <c r="D55" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D55" t="n">
+      <c r="E55" t="n">
         <v>748.9752999999997</v>
       </c>
-      <c r="E55" t="n">
+      <c r="F55" t="n">
         <v>11.69255732819714</v>
       </c>
-      <c r="F55" t="n">
+      <c r="G55" t="n">
         <v>2751.699999999994</v>
       </c>
     </row>
@@ -1773,19 +1940,22 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C56" s="2" t="n">
+          <t>ORANGE</t>
+        </is>
+      </c>
+      <c r="C56" t="b">
+        <v>1</v>
+      </c>
+      <c r="D56" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D56" t="n">
+      <c r="E56" t="n">
         <v>29.95889999999999</v>
       </c>
-      <c r="E56" t="n">
+      <c r="F56" t="n">
         <v>5.800453910614516</v>
       </c>
-      <c r="F56" t="n">
+      <c r="G56" t="n">
         <v>286.4000000000004</v>
       </c>
     </row>
@@ -1800,16 +1970,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C57" s="2" t="n">
+      <c r="C57" t="b">
+        <v>0</v>
+      </c>
+      <c r="D57" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D57" t="n">
+      <c r="E57" t="n">
         <v>164.5709999999999</v>
       </c>
-      <c r="E57" t="n">
+      <c r="F57" t="n">
         <v>5.363471698113191</v>
       </c>
-      <c r="F57" t="n">
+      <c r="G57" t="n">
         <v>1722.500000000002</v>
       </c>
     </row>
@@ -1824,16 +1997,19 @@
           <t>NO_DATA</t>
         </is>
       </c>
-      <c r="C58" s="2" t="n">
+      <c r="C58" t="b">
+        <v>1</v>
+      </c>
+      <c r="D58" s="2" t="n">
         <v>44202</v>
       </c>
-      <c r="D58" t="n">
+      <c r="E58" t="n">
         <v>28.74399999999996</v>
       </c>
-      <c r="E58" t="n">
+      <c r="F58" t="n">
         <v>23.35845864661651</v>
       </c>
-      <c r="F58" t="n">
+      <c r="G58" t="n">
         <v>53.2</v>
       </c>
     </row>
@@ -1848,16 +2024,19 @@
           <t>GREEN</t>
         </is>
       </c>
-      <c r="C59" s="2" t="n">
+      <c r="C59" t="b">
+        <v>0</v>
+      </c>
+      <c r="D59" s="2" t="n">
         <v>44295</v>
       </c>
-      <c r="D59" t="n">
+      <c r="E59" t="n">
         <v>15.61369999999999</v>
       </c>
-      <c r="E59" t="n">
+      <c r="F59" t="n">
         <v>1.69241706161138</v>
       </c>
-      <c r="F59" t="n">
+      <c r="G59" t="n">
         <v>506.3999999999993</v>
       </c>
     </row>
@@ -1872,16 +2051,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C60" s="2" t="n">
+      <c r="C60" t="b">
+        <v>0</v>
+      </c>
+      <c r="D60" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D60" t="n">
+      <c r="E60" t="n">
         <v>440.1059000000001</v>
       </c>
-      <c r="E60" t="n">
+      <c r="F60" t="n">
         <v>15.23231507029302</v>
       </c>
-      <c r="F60" t="n">
+      <c r="G60" t="n">
         <v>1522.199999999998</v>
       </c>
     </row>
@@ -1896,16 +2078,19 @@
           <t>NO_DATA</t>
         </is>
       </c>
-      <c r="C61" s="2" t="n">
+      <c r="C61" t="b">
+        <v>0</v>
+      </c>
+      <c r="D61" s="2" t="n">
         <v>44147</v>
       </c>
-      <c r="D61" t="n">
+      <c r="E61" t="n">
         <v>159.7371999999999</v>
       </c>
-      <c r="E61" t="n">
+      <c r="F61" t="n">
         <v>21.53984479529033</v>
       </c>
-      <c r="F61" t="n">
+      <c r="G61" t="n">
         <v>373.7</v>
       </c>
     </row>
@@ -1920,16 +2105,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C62" s="2" t="n">
+      <c r="C62" t="b">
+        <v>0</v>
+      </c>
+      <c r="D62" s="2" t="n">
         <v>44292</v>
       </c>
-      <c r="D62" t="n">
+      <c r="E62" t="n">
         <v>249.1019</v>
       </c>
-      <c r="E62" t="n">
+      <c r="F62" t="n">
         <v>4.136227614363924</v>
       </c>
-      <c r="F62" t="n">
+      <c r="G62" t="n">
         <v>4310.799999999995</v>
       </c>
     </row>
@@ -1944,16 +2132,19 @@
           <t>GREEN</t>
         </is>
       </c>
-      <c r="C63" s="2" t="n">
+      <c r="C63" t="b">
+        <v>0</v>
+      </c>
+      <c r="D63" s="2" t="n">
         <v>44285</v>
       </c>
-      <c r="D63" t="n">
+      <c r="E63" t="n">
         <v>14.21079999999993</v>
       </c>
-      <c r="E63" t="n">
+      <c r="F63" t="n">
         <v>2.346058091286309</v>
       </c>
-      <c r="F63" t="n">
+      <c r="G63" t="n">
         <v>337.3999999999995</v>
       </c>
     </row>
@@ -1968,16 +2159,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C64" s="2" t="n">
+      <c r="C64" t="b">
+        <v>0</v>
+      </c>
+      <c r="D64" s="2" t="n">
         <v>44291</v>
       </c>
-      <c r="D64" t="n">
+      <c r="E64" t="n">
         <v>449.3274000000005</v>
       </c>
-      <c r="E64" t="n">
+      <c r="F64" t="n">
         <v>8.580054071359964</v>
       </c>
-      <c r="F64" t="n">
+      <c r="G64" t="n">
         <v>2811.099999999999</v>
       </c>
     </row>
@@ -1992,16 +2186,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C65" s="2" t="n">
+      <c r="C65" t="b">
+        <v>0</v>
+      </c>
+      <c r="D65" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D65" t="n">
+      <c r="E65" t="n">
         <v>479.5710999999995</v>
       </c>
-      <c r="E65" t="n">
+      <c r="F65" t="n">
         <v>2.054678691156331</v>
       </c>
-      <c r="F65" t="n">
+      <c r="G65" t="n">
         <v>10589.5</v>
       </c>
     </row>
@@ -2016,16 +2213,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C66" s="2" t="n">
+      <c r="C66" t="b">
+        <v>0</v>
+      </c>
+      <c r="D66" s="2" t="n">
         <v>44295</v>
       </c>
-      <c r="D66" t="n">
+      <c r="E66" t="n">
         <v>348.2129000000001</v>
       </c>
-      <c r="E66" t="n">
+      <c r="F66" t="n">
         <v>4.24428320040222</v>
       </c>
-      <c r="F66" t="n">
+      <c r="G66" t="n">
         <v>4375.700000000006</v>
       </c>
     </row>
@@ -2037,19 +2237,22 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C67" s="2" t="n">
+          <t>ORANGE</t>
+        </is>
+      </c>
+      <c r="C67" t="b">
+        <v>1</v>
+      </c>
+      <c r="D67" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D67" t="n">
+      <c r="E67" t="n">
         <v>20.16499999999996</v>
       </c>
-      <c r="E67" t="n">
+      <c r="F67" t="n">
         <v>4.999810964083223</v>
       </c>
-      <c r="F67" t="n">
+      <c r="G67" t="n">
         <v>211.5999999999985</v>
       </c>
     </row>
@@ -2061,19 +2264,22 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C68" s="2" t="n">
+          <t>ORANGE</t>
+        </is>
+      </c>
+      <c r="C68" t="b">
+        <v>1</v>
+      </c>
+      <c r="D68" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D68" t="n">
+      <c r="E68" t="n">
         <v>16.1713</v>
       </c>
-      <c r="E68" t="n">
+      <c r="F68" t="n">
         <v>41.64675925925939</v>
       </c>
-      <c r="F68" t="n">
+      <c r="G68" t="n">
         <v>21.59999999999993</v>
       </c>
     </row>
@@ -2088,16 +2294,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C69" s="2" t="n">
+      <c r="C69" t="b">
+        <v>0</v>
+      </c>
+      <c r="D69" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D69" t="n">
+      <c r="E69" t="n">
         <v>387.2040000000001</v>
       </c>
-      <c r="E69" t="n">
+      <c r="F69" t="n">
         <v>3.343437276529358</v>
       </c>
-      <c r="F69" t="n">
+      <c r="G69" t="n">
         <v>4614.699999999993</v>
       </c>
     </row>
@@ -2109,19 +2318,22 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C70" s="2" t="n">
+          <t>ORANGE</t>
+        </is>
+      </c>
+      <c r="C70" t="b">
+        <v>1</v>
+      </c>
+      <c r="D70" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D70" t="n">
+      <c r="E70" t="n">
         <v>41.62089999999989</v>
       </c>
-      <c r="E70" t="n">
+      <c r="F70" t="n">
         <v>46.06367265469129</v>
       </c>
-      <c r="F70" t="n">
+      <c r="G70" t="n">
         <v>50.09999999999977</v>
       </c>
     </row>
@@ -2136,16 +2348,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C71" s="2" t="n">
+      <c r="C71" t="b">
+        <v>0</v>
+      </c>
+      <c r="D71" s="2" t="n">
         <v>44292</v>
       </c>
-      <c r="D71" t="n">
+      <c r="E71" t="n">
         <v>715.4720000000001</v>
       </c>
-      <c r="E71" t="n">
+      <c r="F71" t="n">
         <v>26.08978653786225</v>
       </c>
-      <c r="F71" t="n">
+      <c r="G71" t="n">
         <v>1283.600000000001</v>
       </c>
     </row>
@@ -2160,16 +2375,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C72" s="2" t="n">
+      <c r="C72" t="b">
+        <v>0</v>
+      </c>
+      <c r="D72" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D72" t="n">
+      <c r="E72" t="n">
         <v>167.3690999999992</v>
       </c>
-      <c r="E72" t="n">
+      <c r="F72" t="n">
         <v>2.545676421548882</v>
       </c>
-      <c r="F72" t="n">
+      <c r="G72" t="n">
         <v>3478.599999999983</v>
       </c>
     </row>
@@ -2184,16 +2402,19 @@
           <t>NO_DATA</t>
         </is>
       </c>
-      <c r="C73" s="2" t="n">
+      <c r="C73" t="b">
+        <v>1</v>
+      </c>
+      <c r="D73" s="2" t="n">
         <v>44247</v>
       </c>
-      <c r="D73" t="n">
+      <c r="E73" t="n">
         <v>0.3510999999999967</v>
       </c>
-      <c r="E73" t="n">
+      <c r="F73" t="n">
         <v>1.116923076923228</v>
       </c>
-      <c r="F73" t="n">
+      <c r="G73" t="n">
         <v>13.00000000000026</v>
       </c>
     </row>
@@ -2208,16 +2429,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C74" s="2" t="n">
+      <c r="C74" t="b">
+        <v>0</v>
+      </c>
+      <c r="D74" s="2" t="n">
         <v>44291</v>
       </c>
-      <c r="D74" t="n">
+      <c r="E74" t="n">
         <v>226.4898999999999</v>
       </c>
-      <c r="E74" t="n">
+      <c r="F74" t="n">
         <v>4.332142494327985</v>
       </c>
-      <c r="F74" t="n">
+      <c r="G74" t="n">
         <v>2953.100000000006</v>
       </c>
     </row>
@@ -2229,19 +2453,22 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C75" s="2" t="n">
+          <t>ORANGE</t>
+        </is>
+      </c>
+      <c r="C75" t="b">
+        <v>1</v>
+      </c>
+      <c r="D75" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D75" t="n">
+      <c r="E75" t="n">
         <v>4.994300000000021</v>
       </c>
-      <c r="E75" t="n">
+      <c r="F75" t="n">
         <v>6.139339339339324</v>
       </c>
-      <c r="F75" t="n">
+      <c r="G75" t="n">
         <v>33.30000000000002</v>
       </c>
     </row>
@@ -2256,16 +2483,19 @@
           <t>NO_DATA</t>
         </is>
       </c>
-      <c r="C76" s="2" t="n">
+      <c r="C76" t="b">
+        <v>1</v>
+      </c>
+      <c r="D76" s="2" t="n">
         <v>44250</v>
       </c>
-      <c r="D76" t="n">
+      <c r="E76" t="n">
         <v>5.398199999999997</v>
       </c>
-      <c r="E76" t="n">
+      <c r="F76" t="n">
         <v>1.231525015069317</v>
       </c>
-      <c r="F76" t="n">
+      <c r="G76" t="n">
         <v>165.9000000000006</v>
       </c>
     </row>
@@ -2277,19 +2507,22 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C77" s="2" t="n">
+          <t>ORANGE</t>
+        </is>
+      </c>
+      <c r="C77" t="b">
+        <v>1</v>
+      </c>
+      <c r="D77" s="2" t="n">
         <v>44292</v>
       </c>
-      <c r="D77" t="n">
+      <c r="E77" t="n">
         <v>1.808699999999999</v>
       </c>
-      <c r="E77" t="n">
+      <c r="F77" t="n">
         <v>5.598709677419303</v>
       </c>
-      <c r="F77" t="n">
+      <c r="G77" t="n">
         <v>15.49999999999994</v>
       </c>
     </row>
@@ -2304,16 +2537,19 @@
           <t>ORANGE</t>
         </is>
       </c>
-      <c r="C78" s="2" t="n">
+      <c r="C78" t="b">
+        <v>0</v>
+      </c>
+      <c r="D78" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D78" t="n">
+      <c r="E78" t="n">
         <v>58.43169999999991</v>
       </c>
-      <c r="E78" t="n">
+      <c r="F78" t="n">
         <v>2.917507871386316</v>
       </c>
-      <c r="F78" t="n">
+      <c r="G78" t="n">
         <v>1048.099999999999</v>
       </c>
     </row>
@@ -2328,16 +2564,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C79" s="2" t="n">
+      <c r="C79" t="b">
+        <v>0</v>
+      </c>
+      <c r="D79" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D79" t="n">
+      <c r="E79" t="n">
         <v>74.57940000000016</v>
       </c>
-      <c r="E79" t="n">
+      <c r="F79" t="n">
         <v>8.808168843000283</v>
       </c>
-      <c r="F79" t="n">
+      <c r="G79" t="n">
         <v>329.3000000000006</v>
       </c>
     </row>
@@ -2349,19 +2588,22 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C80" s="2" t="n">
+          <t>GREEN</t>
+        </is>
+      </c>
+      <c r="C80" t="b">
+        <v>1</v>
+      </c>
+      <c r="D80" s="2" t="n">
         <v>44291</v>
       </c>
-      <c r="D80" t="n">
+      <c r="E80" t="n">
         <v>0.5850000000000023</v>
       </c>
-      <c r="E80" t="n">
+      <c r="F80" t="n">
         <v>1.703488372092988</v>
       </c>
-      <c r="F80" t="n">
+      <c r="G80" t="n">
         <v>17.20000000000006</v>
       </c>
     </row>
@@ -2376,16 +2618,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C81" s="2" t="n">
+      <c r="C81" t="b">
+        <v>0</v>
+      </c>
+      <c r="D81" s="2" t="n">
         <v>44290</v>
       </c>
-      <c r="D81" t="n">
+      <c r="E81" t="n">
         <v>600.3604000000007</v>
       </c>
-      <c r="E81" t="n">
+      <c r="F81" t="n">
         <v>32.69044762856809</v>
       </c>
-      <c r="F81" t="n">
+      <c r="G81" t="n">
         <v>900.3000000000043</v>
       </c>
     </row>
@@ -2400,16 +2645,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C82" s="2" t="n">
+      <c r="C82" t="b">
+        <v>0</v>
+      </c>
+      <c r="D82" s="2" t="n">
         <v>44292</v>
       </c>
-      <c r="D82" t="n">
+      <c r="E82" t="n">
         <v>193.1476999999999</v>
       </c>
-      <c r="E82" t="n">
+      <c r="F82" t="n">
         <v>4.567616424636942</v>
       </c>
-      <c r="F82" t="n">
+      <c r="G82" t="n">
         <v>1997.000000000003</v>
       </c>
     </row>
@@ -2421,19 +2669,22 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C83" s="2" t="n">
+          <t>ORANGE</t>
+        </is>
+      </c>
+      <c r="C83" t="b">
+        <v>1</v>
+      </c>
+      <c r="D83" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D83" t="n">
+      <c r="E83" t="n">
         <v>10.94490000000005</v>
       </c>
-      <c r="E83" t="n">
+      <c r="F83" t="n">
         <v>7.816939890710488</v>
       </c>
-      <c r="F83" t="n">
+      <c r="G83" t="n">
         <v>91.50000000000063</v>
       </c>
     </row>
@@ -2448,16 +2699,19 @@
           <t>GREEN</t>
         </is>
       </c>
-      <c r="C84" s="2" t="n">
+      <c r="C84" t="b">
+        <v>0</v>
+      </c>
+      <c r="D84" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D84" t="n">
+      <c r="E84" t="n">
         <v>1.866399999999999</v>
       </c>
-      <c r="E84" t="n">
+      <c r="F84" t="n">
         <v>0.3076923076923067</v>
       </c>
-      <c r="F84" t="n">
+      <c r="G84" t="n">
         <v>512.2000000000014</v>
       </c>
     </row>
@@ -2472,16 +2726,19 @@
           <t>NO_DATA</t>
         </is>
       </c>
-      <c r="C85" s="2" t="n">
+      <c r="C85" t="b">
+        <v>0</v>
+      </c>
+      <c r="D85" s="2" t="n">
         <v>44042</v>
       </c>
-      <c r="D85" t="n">
+      <c r="E85" t="n">
         <v>302.7833000000002</v>
       </c>
-      <c r="E85" t="n">
+      <c r="F85" t="n">
         <v>46.47500000000009</v>
       </c>
-      <c r="F85" t="n">
+      <c r="G85" t="n">
         <v>353.6</v>
       </c>
     </row>
@@ -2493,19 +2750,22 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C86" s="2" t="n">
+          <t>ORANGE</t>
+        </is>
+      </c>
+      <c r="C86" t="b">
+        <v>1</v>
+      </c>
+      <c r="D86" s="2" t="n">
         <v>44295</v>
       </c>
-      <c r="D86" t="n">
+      <c r="E86" t="n">
         <v>30.09880000000003</v>
       </c>
-      <c r="E86" t="n">
+      <c r="F86" t="n">
         <v>9.752937378954188</v>
       </c>
-      <c r="F86" t="n">
+      <c r="G86" t="n">
         <v>154.8999999999999</v>
       </c>
     </row>
@@ -2520,16 +2780,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C87" s="2" t="n">
+      <c r="C87" t="b">
+        <v>0</v>
+      </c>
+      <c r="D87" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D87" t="n">
+      <c r="E87" t="n">
         <v>110.5969000000012</v>
       </c>
-      <c r="E87" t="n">
+      <c r="F87" t="n">
         <v>4.410947350485707</v>
       </c>
-      <c r="F87" t="n">
+      <c r="G87" t="n">
         <v>1173.8</v>
       </c>
     </row>
@@ -2544,16 +2807,19 @@
           <t>NO_DATA</t>
         </is>
       </c>
-      <c r="C88" s="2" t="n">
+      <c r="C88" t="b">
+        <v>1</v>
+      </c>
+      <c r="D88" s="2" t="n">
         <v>44281</v>
       </c>
-      <c r="D88" t="n">
+      <c r="E88" t="n">
         <v>357.3109000000004</v>
       </c>
-      <c r="E88" t="n">
+      <c r="F88" t="n">
         <v>121.5519631901843</v>
       </c>
-      <c r="F88" t="n">
+      <c r="G88" t="n">
         <v>162.9999999999995</v>
       </c>
     </row>
@@ -2565,19 +2831,22 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C89" s="2" t="n">
+          <t>RED</t>
+        </is>
+      </c>
+      <c r="C89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D89" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D89" t="n">
+      <c r="E89" t="n">
         <v>130.475</v>
       </c>
-      <c r="E89" t="n">
+      <c r="F89" t="n">
         <v>24.03342135043384</v>
       </c>
-      <c r="F89" t="n">
+      <c r="G89" t="n">
         <v>265.0999999999996</v>
       </c>
     </row>
@@ -2592,16 +2861,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C90" s="2" t="n">
+      <c r="C90" t="b">
+        <v>0</v>
+      </c>
+      <c r="D90" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D90" t="n">
+      <c r="E90" t="n">
         <v>855.1362000000001</v>
       </c>
-      <c r="E90" t="n">
+      <c r="F90" t="n">
         <v>24.77985666046444</v>
       </c>
-      <c r="F90" t="n">
+      <c r="G90" t="n">
         <v>1451.100000000002</v>
       </c>
     </row>
@@ -2616,16 +2888,19 @@
           <t>ORANGE</t>
         </is>
       </c>
-      <c r="C91" s="2" t="n">
+      <c r="C91" t="b">
+        <v>0</v>
+      </c>
+      <c r="D91" s="2" t="n">
         <v>44292</v>
       </c>
-      <c r="D91" t="n">
+      <c r="E91" t="n">
         <v>69.50280000000058</v>
       </c>
-      <c r="E91" t="n">
+      <c r="F91" t="n">
         <v>1.920500988793695</v>
       </c>
-      <c r="F91" t="n">
+      <c r="G91" t="n">
         <v>2123.799999999994</v>
       </c>
     </row>
@@ -2640,16 +2915,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C92" s="2" t="n">
+      <c r="C92" t="b">
+        <v>0</v>
+      </c>
+      <c r="D92" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D92" t="n">
+      <c r="E92" t="n">
         <v>373.4579999999998</v>
       </c>
-      <c r="E92" t="n">
+      <c r="F92" t="n">
         <v>38.35220431151664</v>
       </c>
-      <c r="F92" t="n">
+      <c r="G92" t="n">
         <v>514.9000000000015</v>
       </c>
     </row>
@@ -2664,16 +2942,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C93" s="2" t="n">
+      <c r="C93" t="b">
+        <v>0</v>
+      </c>
+      <c r="D93" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D93" t="n">
+      <c r="E93" t="n">
         <v>620.8080999999999</v>
       </c>
-      <c r="E93" t="n">
+      <c r="F93" t="n">
         <v>26.98895700506782</v>
       </c>
-      <c r="F93" t="n">
+      <c r="G93" t="n">
         <v>1223.4</v>
       </c>
     </row>
@@ -2688,16 +2969,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C94" s="2" t="n">
+      <c r="C94" t="b">
+        <v>0</v>
+      </c>
+      <c r="D94" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D94" t="n">
+      <c r="E94" t="n">
         <v>425.2253999999994</v>
       </c>
-      <c r="E94" t="n">
+      <c r="F94" t="n">
         <v>14.26365560605115</v>
       </c>
-      <c r="F94" t="n">
+      <c r="G94" t="n">
         <v>1606.299999999999</v>
       </c>
     </row>
@@ -2712,16 +2996,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C95" s="2" t="n">
+      <c r="C95" t="b">
+        <v>0</v>
+      </c>
+      <c r="D95" s="2" t="n">
         <v>44295</v>
       </c>
-      <c r="D95" t="n">
+      <c r="E95" t="n">
         <v>361.5248</v>
       </c>
-      <c r="E95" t="n">
+      <c r="F95" t="n">
         <v>19.53416075650114</v>
       </c>
-      <c r="F95" t="n">
+      <c r="G95" t="n">
         <v>846.0000000000036</v>
       </c>
     </row>
@@ -2736,16 +3023,19 @@
           <t>ORANGE</t>
         </is>
       </c>
-      <c r="C96" s="2" t="n">
+      <c r="C96" t="b">
+        <v>0</v>
+      </c>
+      <c r="D96" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D96" t="n">
+      <c r="E96" t="n">
         <v>82.14779999999992</v>
       </c>
-      <c r="E96" t="n">
+      <c r="F96" t="n">
         <v>2.888041557707264</v>
       </c>
-      <c r="F96" t="n">
+      <c r="G96" t="n">
         <v>1414.9</v>
       </c>
     </row>
@@ -2760,16 +3050,19 @@
           <t>GREEN</t>
         </is>
       </c>
-      <c r="C97" s="2" t="n">
+      <c r="C97" t="b">
+        <v>0</v>
+      </c>
+      <c r="D97" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D97" t="n">
+      <c r="E97" t="n">
         <v>15.49539999999999</v>
       </c>
-      <c r="E97" t="n">
+      <c r="F97" t="n">
         <v>2.153116691285081</v>
       </c>
-      <c r="F97" t="n">
+      <c r="G97" t="n">
         <v>338.4999999999991</v>
       </c>
     </row>
@@ -2784,16 +3077,19 @@
           <t>ORANGE</t>
         </is>
       </c>
-      <c r="C98" s="2" t="n">
+      <c r="C98" t="b">
+        <v>0</v>
+      </c>
+      <c r="D98" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D98" t="n">
+      <c r="E98" t="n">
         <v>29.04009999999998</v>
       </c>
-      <c r="E98" t="n">
+      <c r="F98" t="n">
         <v>1.364687422578243</v>
       </c>
-      <c r="F98" t="n">
+      <c r="G98" t="n">
         <v>1210.900000000004</v>
       </c>
     </row>
@@ -2805,19 +3101,22 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C99" s="2" t="n">
+          <t>ORANGE</t>
+        </is>
+      </c>
+      <c r="C99" t="b">
+        <v>1</v>
+      </c>
+      <c r="D99" s="2" t="n">
         <v>44295</v>
       </c>
-      <c r="D99" t="n">
+      <c r="E99" t="n">
         <v>5.440800000000036</v>
       </c>
-      <c r="E99" t="n">
+      <c r="F99" t="n">
         <v>4.325088967971564</v>
       </c>
-      <c r="F99" t="n">
+      <c r="G99" t="n">
         <v>56.20000000000012</v>
       </c>
     </row>
@@ -2832,16 +3131,19 @@
           <t>NO_DATA</t>
         </is>
       </c>
-      <c r="C100" s="2" t="n">
+      <c r="C100" t="b">
+        <v>0</v>
+      </c>
+      <c r="D100" s="2" t="n">
         <v>44277</v>
       </c>
-      <c r="D100" t="n">
+      <c r="E100" t="n">
         <v>6.033799999999974</v>
       </c>
-      <c r="E100" t="n">
+      <c r="F100" t="n">
         <v>0.03566684552554732</v>
       </c>
-      <c r="F100" t="n">
+      <c r="G100" t="n">
         <v>8386.5</v>
       </c>
     </row>
@@ -2856,16 +3158,19 @@
           <t>NO_DATA</t>
         </is>
       </c>
-      <c r="C101" s="2" t="n">
+      <c r="C101" t="b">
+        <v>1</v>
+      </c>
+      <c r="D101" s="2" t="n">
         <v>44270</v>
       </c>
-      <c r="D101" t="n">
+      <c r="E101" t="n">
         <v>33.77939999999999</v>
       </c>
-      <c r="E101" t="n">
+      <c r="F101" t="n">
         <v>6.582950333580418</v>
       </c>
-      <c r="F101" t="n">
+      <c r="G101" t="n">
         <v>269.8000000000008</v>
       </c>
     </row>
@@ -2880,16 +3185,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C102" s="2" t="n">
+      <c r="C102" t="b">
+        <v>0</v>
+      </c>
+      <c r="D102" s="2" t="n">
         <v>44289</v>
       </c>
-      <c r="D102" t="n">
+      <c r="E102" t="n">
         <v>833.2896999999997</v>
       </c>
-      <c r="E102" t="n">
+      <c r="F102" t="n">
         <v>22.43802264808363</v>
       </c>
-      <c r="F102" t="n">
+      <c r="G102" t="n">
         <v>1607.2</v>
       </c>
     </row>
@@ -2901,19 +3209,22 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C103" s="2" t="n">
+          <t>GREEN</t>
+        </is>
+      </c>
+      <c r="C103" t="b">
+        <v>1</v>
+      </c>
+      <c r="D103" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D103" t="n">
+      <c r="E103" t="n">
         <v>2.447800000000007</v>
       </c>
-      <c r="E103" t="n">
+      <c r="F103" t="n">
         <v>2.207058823529407</v>
       </c>
-      <c r="F103" t="n">
+      <c r="G103" t="n">
         <v>42.50000000000007</v>
       </c>
     </row>
@@ -2928,16 +3239,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C104" s="2" t="n">
+      <c r="C104" t="b">
+        <v>0</v>
+      </c>
+      <c r="D104" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D104" t="n">
+      <c r="E104" t="n">
         <v>240.8949000000008</v>
       </c>
-      <c r="E104" t="n">
+      <c r="F104" t="n">
         <v>0.3229003980201981</v>
       </c>
-      <c r="F104" t="n">
+      <c r="G104" t="n">
         <v>33013.4</v>
       </c>
     </row>
@@ -2952,16 +3266,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C105" s="2" t="n">
+      <c r="C105" t="b">
+        <v>0</v>
+      </c>
+      <c r="D105" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D105" t="n">
+      <c r="E105" t="n">
         <v>664.8125</v>
       </c>
-      <c r="E105" t="n">
+      <c r="F105" t="n">
         <v>23.9191381198185</v>
       </c>
-      <c r="F105" t="n">
+      <c r="G105" t="n">
         <v>1278.600000000006</v>
       </c>
     </row>
@@ -2976,16 +3293,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C106" s="2" t="n">
+      <c r="C106" t="b">
+        <v>0</v>
+      </c>
+      <c r="D106" s="2" t="n">
         <v>44290</v>
       </c>
-      <c r="D106" t="n">
+      <c r="E106" t="n">
         <v>766.2236999999993</v>
       </c>
-      <c r="E106" t="n">
+      <c r="F106" t="n">
         <v>13.60965024094511</v>
       </c>
-      <c r="F106" t="n">
+      <c r="G106" t="n">
         <v>3216.5</v>
       </c>
     </row>
@@ -2997,19 +3317,22 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C107" s="2" t="n">
+          <t>ORANGE</t>
+        </is>
+      </c>
+      <c r="C107" t="b">
+        <v>1</v>
+      </c>
+      <c r="D107" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D107" t="n">
+      <c r="E107" t="n">
         <v>24.77429999999999</v>
       </c>
-      <c r="E107" t="n">
+      <c r="F107" t="n">
         <v>8.075755102040818</v>
       </c>
-      <c r="F107" t="n">
+      <c r="G107" t="n">
         <v>122.5000000000001</v>
       </c>
     </row>
@@ -3021,19 +3344,22 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C108" s="2" t="n">
+          <t>GREEN</t>
+        </is>
+      </c>
+      <c r="C108" t="b">
+        <v>1</v>
+      </c>
+      <c r="D108" s="2" t="n">
         <v>44290</v>
       </c>
-      <c r="D108" t="n">
+      <c r="E108" t="n">
         <v>5.5745</v>
       </c>
-      <c r="E108" t="n">
+      <c r="F108" t="n">
         <v>3.145951035781552</v>
       </c>
-      <c r="F108" t="n">
+      <c r="G108" t="n">
         <v>159.2999999999996</v>
       </c>
     </row>
@@ -3048,16 +3374,19 @@
           <t>ORANGE</t>
         </is>
       </c>
-      <c r="C109" s="2" t="n">
+      <c r="C109" t="b">
+        <v>0</v>
+      </c>
+      <c r="D109" s="2" t="n">
         <v>44292</v>
       </c>
-      <c r="D109" t="n">
+      <c r="E109" t="n">
         <v>30.51109999999999</v>
       </c>
-      <c r="E109" t="n">
+      <c r="F109" t="n">
         <v>3.946407624633434</v>
       </c>
-      <c r="F109" t="n">
+      <c r="G109" t="n">
         <v>409.1999999999999</v>
       </c>
     </row>
@@ -3072,16 +3401,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C110" s="2" t="n">
+      <c r="C110" t="b">
+        <v>0</v>
+      </c>
+      <c r="D110" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D110" t="n">
+      <c r="E110" t="n">
         <v>180.1903000000002</v>
       </c>
-      <c r="E110" t="n">
+      <c r="F110" t="n">
         <v>26.96502157497308</v>
       </c>
-      <c r="F110" t="n">
+      <c r="G110" t="n">
         <v>370.7999999999998</v>
       </c>
     </row>
@@ -3096,16 +3428,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C111" s="2" t="n">
+      <c r="C111" t="b">
+        <v>0</v>
+      </c>
+      <c r="D111" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D111" t="n">
+      <c r="E111" t="n">
         <v>759.8352999999995</v>
       </c>
-      <c r="E111" t="n">
+      <c r="F111" t="n">
         <v>19.37753296008665</v>
       </c>
-      <c r="F111" t="n">
+      <c r="G111" t="n">
         <v>2214.800000000002</v>
       </c>
     </row>
@@ -3117,19 +3452,22 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C112" s="2" t="n">
+          <t>GREEN</t>
+        </is>
+      </c>
+      <c r="C112" t="b">
+        <v>1</v>
+      </c>
+      <c r="D112" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D112" t="n">
+      <c r="E112" t="n">
         <v>0.1469000000000001</v>
       </c>
-      <c r="E112" t="n">
+      <c r="F112" t="n">
         <v>0.2850340136054444</v>
       </c>
-      <c r="F112" t="n">
+      <c r="G112" t="n">
         <v>14.70000000000002</v>
       </c>
     </row>
@@ -3141,19 +3479,22 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C113" s="2" t="n">
+          <t>GREEN</t>
+        </is>
+      </c>
+      <c r="C113" t="b">
+        <v>1</v>
+      </c>
+      <c r="D113" s="2" t="n">
         <v>44292</v>
       </c>
-      <c r="D113" t="n">
+      <c r="E113" t="n">
         <v>0.7564000000000078</v>
       </c>
-      <c r="E113" t="n">
+      <c r="F113" t="n">
         <v>1.172289156626519</v>
       </c>
-      <c r="F113" t="n">
+      <c r="G113" t="n">
         <v>33.20000000000007</v>
       </c>
     </row>
@@ -3168,16 +3509,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C114" s="2" t="n">
+      <c r="C114" t="b">
+        <v>0</v>
+      </c>
+      <c r="D114" s="2" t="n">
         <v>44295</v>
       </c>
-      <c r="D114" t="n">
+      <c r="E114" t="n">
         <v>482.1491999999998</v>
       </c>
-      <c r="E114" t="n">
+      <c r="F114" t="n">
         <v>32.93082237279114</v>
       </c>
-      <c r="F114" t="n">
+      <c r="G114" t="n">
         <v>752.7000000000015</v>
       </c>
     </row>
@@ -3192,16 +3536,19 @@
           <t>DARKRED</t>
         </is>
       </c>
-      <c r="C115" s="2" t="n">
+      <c r="C115" t="b">
+        <v>0</v>
+      </c>
+      <c r="D115" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D115" t="n">
+      <c r="E115" t="n">
         <v>1359.8075</v>
       </c>
-      <c r="E115" t="n">
+      <c r="F115" t="n">
         <v>26.6420860585198</v>
       </c>
-      <c r="F115" t="n">
+      <c r="G115" t="n">
         <v>2905.000000000001</v>
       </c>
     </row>
@@ -3216,16 +3563,19 @@
           <t>RED</t>
         </is>
       </c>
-      <c r="C116" s="2" t="n">
+      <c r="C116" t="b">
+        <v>0</v>
+      </c>
+      <c r="D116" s="2" t="n">
         <v>44292</v>
       </c>
-      <c r="D116" t="n">
+      <c r="E116" t="n">
         <v>282.3928999999989</v>
       </c>
-      <c r="E116" t="n">
+      <c r="F116" t="n">
         <v>7.682510373443965</v>
       </c>
-      <c r="F116" t="n">
+      <c r="G116" t="n">
         <v>1927.999999999997</v>
       </c>
     </row>
@@ -3240,16 +3590,19 @@
           <t>NO_DATA</t>
         </is>
       </c>
-      <c r="C117" s="2" t="n">
+      <c r="C117" t="b">
+        <v>1</v>
+      </c>
+      <c r="D117" s="2" t="n">
         <v>44115</v>
       </c>
-      <c r="D117" t="n">
+      <c r="E117" t="n">
         <v>0.1048000000000002</v>
       </c>
-      <c r="E117" t="n">
+      <c r="F117" t="n">
         <v>0.3578651685393244</v>
       </c>
-      <c r="F117" t="n">
+      <c r="G117" t="n">
         <v>17.80000000000008</v>
       </c>
     </row>
@@ -3261,19 +3614,22 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C118" s="2" t="n">
+          <t>ORANGE</t>
+        </is>
+      </c>
+      <c r="C118" t="b">
+        <v>1</v>
+      </c>
+      <c r="D118" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D118" t="n">
+      <c r="E118" t="n">
         <v>21.9648000000001</v>
       </c>
-      <c r="E118" t="n">
+      <c r="F118" t="n">
         <v>4.515257731958902</v>
       </c>
-      <c r="F118" t="n">
+      <c r="G118" t="n">
         <v>242.4999999999983</v>
       </c>
     </row>
@@ -3285,19 +3641,22 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C119" s="2" t="n">
+          <t>GREEN</t>
+        </is>
+      </c>
+      <c r="C119" t="b">
+        <v>1</v>
+      </c>
+      <c r="D119" s="2" t="n">
         <v>44294</v>
       </c>
-      <c r="D119" t="n">
+      <c r="E119" t="n">
         <v>11.73310000000001</v>
       </c>
-      <c r="E119" t="n">
+      <c r="F119" t="n">
         <v>3.762177470106986</v>
       </c>
-      <c r="F119" t="n">
+      <c r="G119" t="n">
         <v>158.8999999999999</v>
       </c>
     </row>
@@ -3309,19 +3668,22 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>TOO_LOW_TESTING</t>
-        </is>
-      </c>
-      <c r="C120" s="2" t="n">
+          <t>GREEN</t>
+        </is>
+      </c>
+      <c r="C120" t="b">
+        <v>1</v>
+      </c>
+      <c r="D120" s="2" t="n">
         <v>44293</v>
       </c>
-      <c r="D120" t="n">
+      <c r="E120" t="n">
         <v>3.135400000000027</v>
       </c>
-      <c r="E120" t="n">
+      <c r="F120" t="n">
         <v>3.050683229813664</v>
       </c>
-      <c r="F120" t="n">
+      <c r="G120" t="n">
         <v>80.49999999999997</v>
       </c>
     </row>
@@ -3336,14 +3698,17 @@
           <t>NO_DATA</t>
         </is>
       </c>
-      <c r="C121" t="inlineStr"/>
-      <c r="D121" t="n">
-        <v>0</v>
-      </c>
+      <c r="C121" t="b">
+        <v>1</v>
+      </c>
+      <c r="D121" t="inlineStr"/>
       <c r="E121" t="n">
         <v>0</v>
       </c>
       <c r="F121" t="n">
+        <v>0</v>
+      </c>
+      <c r="G121" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>